<commit_message>
errors corrected in gold standard
</commit_message>
<xml_diff>
--- a/manual_download/Amt für Statistik Berlin-Brandenburg/AP_Geschaeftsbericht_DE_2017_BBB.xlsx
+++ b/manual_download/Amt für Statistik Berlin-Brandenburg/AP_Geschaeftsbericht_DE_2017_BBB.xlsx
@@ -376,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -734,7 +734,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>